<commit_message>
test cases for Sicom
</commit_message>
<xml_diff>
--- a/Popeyes.suite/Resources/Sicom.xlsx
+++ b/Popeyes.suite/Resources/Sicom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -58,73 +58,70 @@
     <t xml:space="preserve">Drink</t>
   </si>
   <si>
-    <t xml:space="preserve">Butterfly Shrimp &amp; Tender Combo</t>
+    <t xml:space="preserve">SPICY CHICKEN SANDWICH</t>
   </si>
   <si>
     <t xml:space="preserve">Dine In</t>
   </si>
   <si>
-    <t xml:space="preserve">Sandwiches Seafood, To Seafood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BFLY SHRIMP&amp;TENDER</t>
+    <t xml:space="preserve">SANDWICHES &amp; SEAFOOD, COMBO</t>
   </si>
   <si>
     <t xml:space="preserve">Combo</t>
   </si>
   <si>
-    <t xml:space="preserve">Bfly Shr &amp; 2Tnd Comb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLASSIC, BBQ SAUCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mash Gravy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CocaCola</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chicken Tender 3 PC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chicken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3PC Tender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3PC Tender Combo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLASSIC, BUFFALO SAUCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cajun Rice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DietCoke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kids Mac &amp; Cheese</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combos Kids, To Kids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mac Cheese Kids Meal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H.Mac&amp;Cheese KD Meal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strawberry Cheesecake Cup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desserts Sides</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stwbry CC Cup</t>
+    <t xml:space="preserve">Spcy San CMB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Fries Reg, HOMESTYLE MAC &amp; CHEESE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Rg Coke, CHILLED MANGO LEMONADE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4PC BIC COMBO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHICKEN, 4PC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL WHITE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4PC BIC Combo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Mash&amp;Gravy Re, CAJUN FRIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Rg Coke, OrangeFanta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHRIMP AND 2 TENDERS COMBO CUST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SANDWICHES &amp; SEAFOOD, TO SANDWICHES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMBO, BTTRFLY SHRIMP &amp; TENDERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSHRIMP&amp;TND C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Cocktail, BLACKENED RANCH SAUCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*BBQ, BTTRMLK RANCH SAUCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Tndr Clsc, Spicy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Rg Coke, DietCoke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHRIMP AND 2 TENDERS COMBO</t>
   </si>
   <si>
     <t xml:space="preserve">12P WINGS LARGE COMBO</t>
@@ -358,8 +355,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -367,13 +364,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="49.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="38.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="25.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="25.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -428,23 +425,19 @@
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -452,32 +445,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -485,19 +474,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -505,19 +509,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -525,32 +526,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
adde imgaes and amend SicomTests script
</commit_message>
<xml_diff>
--- a/Popeyes.suite/Resources/Sicom.xlsx
+++ b/Popeyes.suite/Resources/Sicom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">SANDWICHES &amp; SEAFOOD, COMBO</t>
   </si>
   <si>
-    <t xml:space="preserve">Combo</t>
+    <t xml:space="preserve">COMBO</t>
   </si>
   <si>
     <t xml:space="preserve">Spcy San CMB</t>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">*BBQ, BTTRMLK RANCH SAUCE</t>
   </si>
   <si>
-    <t xml:space="preserve">*Tndr Clsc, Spicy</t>
+    <t xml:space="preserve">*Tndr Clsc, SPICY</t>
   </si>
   <si>
     <t xml:space="preserve">*Rg Coke, DietCoke</t>
@@ -356,7 +356,7 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -485,6 +485,9 @@
       <c r="E4" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>28</v>
       </c>
@@ -520,6 +523,9 @@
       <c r="E5" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -536,6 +542,9 @@
       </c>
       <c r="E6" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Amendements on the scripts and starting testing all the mealoption
</commit_message>
<xml_diff>
--- a/Popeyes.suite/Resources/Sicom.xlsx
+++ b/Popeyes.suite/Resources/Sicom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="64">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -31,12 +31,12 @@
     <t xml:space="preserve">DineOption</t>
   </si>
   <si>
+    <t xml:space="preserve">SelectMeal</t>
+  </si>
+  <si>
     <t xml:space="preserve">MainCourse</t>
   </si>
   <si>
-    <t xml:space="preserve">SelectMeal</t>
-  </si>
-  <si>
     <t xml:space="preserve">SelectMealOption</t>
   </si>
   <si>
@@ -58,94 +58,160 @@
     <t xml:space="preserve">Drink</t>
   </si>
   <si>
+    <t xml:space="preserve">SPICY CHICKEN SANDWICH ALA CARTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dine In</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SANDWICHES &amp; SEAFOOD</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPICY CHICKEN SANDWICH</t>
   </si>
   <si>
-    <t xml:space="preserve">Dine In</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SANDWICHES &amp; SEAFOOD, COMBO</t>
+    <t xml:space="preserve">SANDWICH ONLY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spcy San CMB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Fries Reg, HOMESTYLE MAC &amp; CHEESE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Rg Coke, CHILLED MANGO LEMONADE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPICY CHICKEN SANDWICH DINNER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DINNER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPICY CHICKEN SANDWICH COMBO</t>
   </si>
   <si>
     <t xml:space="preserve">COMBO</t>
   </si>
   <si>
-    <t xml:space="preserve">Spcy San CMB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Fries Reg, HOMESTYLE MAC &amp; CHEESE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Rg Coke, CHILLED MANGO LEMONADE</t>
+    <t xml:space="preserve">SPICY CHICKEN SANDWICH LARGE COMBO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LARGE COMBO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4PC BIC ALA CARTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHICKEN, 4PC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL WHITE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALA CARTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4PC BIC Combo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Mash&amp;Gravy Re, CAJUN FRIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Rg Coke, OrangeFanta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4PC BIC DINNER</t>
   </si>
   <si>
     <t xml:space="preserve">4PC BIC COMBO</t>
   </si>
   <si>
-    <t xml:space="preserve">CHICKEN, 4PC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALL WHITE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4PC BIC Combo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Mash&amp;Gravy Re, CAJUN FRIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Rg Coke, OrangeFanta</t>
+    <t xml:space="preserve">4PC BIC LARGE COMBO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHRIMP AND 2 TENDERS ALA CARTE CUST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SANDWICHES &amp; SEAFOOD, TO SANDWICHES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMBO, BTTRFLY SHRIMP &amp; TENDERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A LA CARTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSHRIMP&amp;TND C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Cocktail, BLACKENED RANCH SAUCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*BBQ, BTTRMLK RANCH SAUCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Tndr Clsc, SPICY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Rg Coke, DietCoke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHRIMP AND 2 TENDERS DINNER CUST</t>
   </si>
   <si>
     <t xml:space="preserve">SHRIMP AND 2 TENDERS COMBO CUST</t>
   </si>
   <si>
-    <t xml:space="preserve">SANDWICHES &amp; SEAFOOD, TO SANDWICHES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBO, BTTRFLY SHRIMP &amp; TENDERS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BSHRIMP&amp;TND C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Cocktail, BLACKENED RANCH SAUCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*BBQ, BTTRMLK RANCH SAUCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Tndr Clsc, SPICY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Rg Coke, DietCoke</t>
+    <t xml:space="preserve">SHRIMP AND 2 TENDERS LARGE COMBO CUST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHRIMP AND 2 TENDERS ALA CARTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHRIMP AND 2 TENDERS DINNER</t>
   </si>
   <si>
     <t xml:space="preserve">SHRIMP AND 2 TENDERS COMBO</t>
   </si>
   <si>
+    <t xml:space="preserve">SHRIMP AND 2 TENDERS LARGE COMBO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12P WINGS ALA CARTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WINGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6P SWEET N’ SPICY WINGS, 6P HONEY BBQ WINGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12P WINGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LgCmb 12P WNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Btrmlk Ranch, BBQ SAUCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Btrmlk Ranch, BUFFALO SAUCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Mash&amp;Gravy Re, COLESLAW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Lg Coke, SicomDrPepper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12P WINGS DINNER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12P WINGS COMBO</t>
+  </si>
+  <si>
     <t xml:space="preserve">12P WINGS LARGE COMBO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WINGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6P SWEET N’ SPICY WINGS, 6P HONEY BBQ WINGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LgCmb 12P WNG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Btrmlk Ranch, BBQ SAUCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Btrmlk Ranch, BUFFALO SAUCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Mash&amp;Gravy Re, COLESLAW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Lg Coke, SicomDrPepper</t>
   </si>
 </sst>
 </file>
@@ -161,7 +227,6 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -353,10 +418,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1048576"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -373,7 +438,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="25.68"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -411,7 +476,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
@@ -425,144 +490,584 @@
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="1" t="s">
+      <c r="F16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
changes on the script
</commit_message>
<xml_diff>
--- a/Popeyes.suite/Resources/Sicom.xlsx
+++ b/Popeyes.suite/Resources/Sicom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="75">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -73,34 +73,43 @@
     <t xml:space="preserve">SANDWICH ONLY</t>
   </si>
   <si>
+    <t xml:space="preserve">Spicy San</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPICY CHICKEN SANDWICH DINNER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DINNER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spcy San DNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Fries Reg, HOMESTYLE MAC &amp; CHEESE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPICY CHICKEN SANDWICH COMBO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMBO</t>
+  </si>
+  <si>
     <t xml:space="preserve">Spcy San CMB</t>
   </si>
   <si>
-    <t xml:space="preserve">*Fries Reg, HOMESTYLE MAC &amp; CHEESE</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Rg Coke, CHILLED MANGO LEMONADE</t>
   </si>
   <si>
-    <t xml:space="preserve">SPICY CHICKEN SANDWICH DINNER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DINNER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPICY CHICKEN SANDWICH COMBO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBO</t>
-  </si>
-  <si>
     <t xml:space="preserve">SPICY CHICKEN SANDWICH LARGE COMBO</t>
   </si>
   <si>
     <t xml:space="preserve">LARGE COMBO</t>
   </si>
   <si>
-    <t xml:space="preserve">4PC BIC ALA CARTE</t>
+    <t xml:space="preserve">Spcy San LCMB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4PC BIC DINNER</t>
   </si>
   <si>
     <t xml:space="preserve">CHICKEN, 4PC</t>
@@ -109,31 +118,34 @@
     <t xml:space="preserve">ALL WHITE</t>
   </si>
   <si>
-    <t xml:space="preserve">ALA CARTE</t>
+    <t xml:space="preserve">4PC BIC Dinne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Biscuit, FRIED PICKLES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Mash&amp;Gravy Re, CAJUN FRIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4PC BIC COMBO</t>
   </si>
   <si>
     <t xml:space="preserve">4PC BIC Combo</t>
   </si>
   <si>
-    <t xml:space="preserve">*Mash&amp;Gravy Re, CAJUN FRIES</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Rg Coke, OrangeFanta</t>
   </si>
   <si>
-    <t xml:space="preserve">4PC BIC DINNER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4PC BIC COMBO</t>
-  </si>
-  <si>
     <t xml:space="preserve">4PC BIC LARGE COMBO</t>
   </si>
   <si>
+    <t xml:space="preserve">LgCmb 4PC BIC</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHRIMP AND 2 TENDERS ALA CARTE CUST</t>
   </si>
   <si>
-    <t xml:space="preserve">SANDWICHES &amp; SEAFOOD, TO SANDWICHES</t>
+    <t xml:space="preserve">SANDWICHES &amp; SEAFOOD, TO SEAFOOD</t>
   </si>
   <si>
     <t xml:space="preserve">COMBO, BTTRFLY SHRIMP &amp; TENDERS</t>
@@ -142,30 +154,45 @@
     <t xml:space="preserve">A LA CARTE</t>
   </si>
   <si>
+    <t xml:space="preserve">BSHRIMP&amp;TENDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Cocktail, PICKLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*BBQ, BTTRMLK RANCH SAUCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Tndr Clsc, SPICY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHRIMP AND 2 TENDERS DINNER CUST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSHRIMP&amp;TND D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Cocktail, TARTAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*BBQ, SWEET HEAT SAUCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Mash&amp;Gravy Re, RED BEAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHRIMP AND 2 TENDERS COMBO CUST</t>
+  </si>
+  <si>
     <t xml:space="preserve">BSHRIMP&amp;TND C</t>
   </si>
   <si>
     <t xml:space="preserve">*Cocktail, BLACKENED RANCH SAUCE</t>
   </si>
   <si>
-    <t xml:space="preserve">*BBQ, BTTRMLK RANCH SAUCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Tndr Clsc, SPICY</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Rg Coke, DietCoke</t>
   </si>
   <si>
-    <t xml:space="preserve">SHRIMP AND 2 TENDERS DINNER CUST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHRIMP AND 2 TENDERS COMBO CUST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHRIMP AND 2 TENDERS LARGE COMBO CUST</t>
-  </si>
-  <si>
     <t xml:space="preserve">SHRIMP AND 2 TENDERS ALA CARTE</t>
   </si>
   <si>
@@ -175,10 +202,7 @@
     <t xml:space="preserve">SHRIMP AND 2 TENDERS COMBO</t>
   </si>
   <si>
-    <t xml:space="preserve">SHRIMP AND 2 TENDERS LARGE COMBO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12P WINGS ALA CARTE</t>
+    <t xml:space="preserve">12P WINGS</t>
   </si>
   <si>
     <t xml:space="preserve">WINGS</t>
@@ -187,31 +211,40 @@
     <t xml:space="preserve">6P SWEET N’ SPICY WINGS, 6P HONEY BBQ WINGS</t>
   </si>
   <si>
-    <t xml:space="preserve">12P WINGS</t>
+    <t xml:space="preserve">12P WNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Btrmlk Ranch, BBQ SAUCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Btrmlk Ranch, BUFFALO SAUCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12P WINGS DINNER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12P  WNG DIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Fries Reg, FRIED PICKLES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12P WINGS COMBO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12P WNG Cmb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12P WINGS LARGE COMBO</t>
   </si>
   <si>
     <t xml:space="preserve">LgCmb 12P WNG</t>
   </si>
   <si>
-    <t xml:space="preserve">*Btrmlk Ranch, BBQ SAUCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Btrmlk Ranch, BUFFALO SAUCE</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Mash&amp;Gravy Re, COLESLAW</t>
   </si>
   <si>
     <t xml:space="preserve">*Lg Coke, SicomDrPepper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12P WINGS DINNER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12P WINGS COMBO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12P WINGS LARGE COMBO</t>
   </si>
 </sst>
 </file>
@@ -418,10 +451,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -498,19 +531,13 @@
       <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
@@ -522,16 +549,13 @@
         <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -554,13 +578,13 @@
         <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,7 +592,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -580,10 +604,10 @@
         <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,28 +615,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -620,28 +644,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,28 +673,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -678,22 +696,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -701,37 +728,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -739,113 +763,83 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L12" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -853,22 +847,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -876,22 +870,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>40</v>
+        <v>63</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -899,22 +899,31 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>40</v>
+        <v>67</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -922,22 +931,34 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -945,129 +966,39 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Made some changes on the scripts
</commit_message>
<xml_diff>
--- a/Popeyes.suite/Resources/Sicom.xlsx
+++ b/Popeyes.suite/Resources/Sicom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="71">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -43,16 +43,10 @@
     <t xml:space="preserve">MealDisplayName</t>
   </si>
   <si>
-    <t xml:space="preserve">Flavor1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flavor2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sides1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sides2</t>
+    <t xml:space="preserve">Flavors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sides</t>
   </si>
   <si>
     <t xml:space="preserve">Drink</t>
@@ -73,7 +67,7 @@
     <t xml:space="preserve">SANDWICH ONLY</t>
   </si>
   <si>
-    <t xml:space="preserve">Spicy San</t>
+    <t xml:space="preserve">Spicy Sand</t>
   </si>
   <si>
     <t xml:space="preserve">SPICY CHICKEN SANDWICH DINNER</t>
@@ -85,7 +79,7 @@
     <t xml:space="preserve">Spcy San DNR</t>
   </si>
   <si>
-    <t xml:space="preserve">*Fries Reg, HOMESTYLE MAC &amp; CHEESE</t>
+    <t xml:space="preserve">Fries Reg, HOMESTYLE MAC &amp; CHEESE</t>
   </si>
   <si>
     <t xml:space="preserve">SPICY CHICKEN SANDWICH COMBO</t>
@@ -97,7 +91,7 @@
     <t xml:space="preserve">Spcy San CMB</t>
   </si>
   <si>
-    <t xml:space="preserve">*Rg Coke, CHILLED MANGO LEMONADE</t>
+    <t xml:space="preserve">Rg Coke, CHILLED MANGO LEMONADE</t>
   </si>
   <si>
     <t xml:space="preserve">SPICY CHICKEN SANDWICH LARGE COMBO</t>
@@ -118,13 +112,10 @@
     <t xml:space="preserve">ALL WHITE</t>
   </si>
   <si>
-    <t xml:space="preserve">4PC BIC Dinne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Biscuit, FRIED PICKLES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Mash&amp;Gravy Re, CAJUN FRIES</t>
+    <t xml:space="preserve">4PC BIC Dinner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biscuit, FRIED PICKLES, Mash&amp;Gravy Re, CAJUN FRIES</t>
   </si>
   <si>
     <t xml:space="preserve">4PC BIC COMBO</t>
@@ -133,7 +124,10 @@
     <t xml:space="preserve">4PC BIC Combo</t>
   </si>
   <si>
-    <t xml:space="preserve">*Rg Coke, OrangeFanta</t>
+    <t xml:space="preserve">Mash&amp;Gravy Re, CAJUN FRIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rg Coke, OrangeFanta</t>
   </si>
   <si>
     <t xml:space="preserve">4PC BIC LARGE COMBO</t>
@@ -154,43 +148,40 @@
     <t xml:space="preserve">A LA CARTE</t>
   </si>
   <si>
-    <t xml:space="preserve">BSHRIMP&amp;TENDE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Cocktail, PICKLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*BBQ, BTTRMLK RANCH SAUCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Tndr Clsc, SPICY</t>
+    <t xml:space="preserve">BSHRIMP&amp;TENDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cocktail, PICKLE, BBQ, BTTRMLK RANCH SAUCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tndr Clsc, SPICY</t>
   </si>
   <si>
     <t xml:space="preserve">SHRIMP AND 2 TENDERS DINNER CUST</t>
   </si>
   <si>
-    <t xml:space="preserve">BSHRIMP&amp;TND D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Cocktail, TARTAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*BBQ, SWEET HEAT SAUCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Mash&amp;Gravy Re, RED BEAN</t>
+    <t xml:space="preserve">BSHRIMP&amp;TND DNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cocktail, TARTAR, BBQ, SWEET HEAT SAUCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tndr Clsc, SPICY, Mash&amp;Gravy Re, RED BEAN</t>
   </si>
   <si>
     <t xml:space="preserve">SHRIMP AND 2 TENDERS COMBO CUST</t>
   </si>
   <si>
-    <t xml:space="preserve">BSHRIMP&amp;TND C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Cocktail, BLACKENED RANCH SAUCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Rg Coke, DietCoke</t>
+    <t xml:space="preserve">BSHRIMP&amp;TND CMB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cocktail, BLACKENED RANCH SAUCE, BBQ, BTTRMLK RANCH SAUCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tndr Clsc, SPICY, Mash&amp;Gravy Re, CAJUN FRIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rg Coke, DietCoke</t>
   </si>
   <si>
     <t xml:space="preserve">SHRIMP AND 2 TENDERS ALA CARTE</t>
@@ -208,16 +199,13 @@
     <t xml:space="preserve">WINGS</t>
   </si>
   <si>
-    <t xml:space="preserve">6P SWEET N’ SPICY WINGS, 6P HONEY BBQ WINGS</t>
+    <t xml:space="preserve">6P HONEY LEMON WINGS, 6P HONEY BBQ WINGS</t>
   </si>
   <si>
     <t xml:space="preserve">12P WNG</t>
   </si>
   <si>
-    <t xml:space="preserve">*Btrmlk Ranch, BBQ SAUCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Btrmlk Ranch, BUFFALO SAUCE</t>
+    <t xml:space="preserve">Btrmlk Ranch, BBQ SAUCE, Btrmlk Ranch, BUFFALO SAUCE</t>
   </si>
   <si>
     <t xml:space="preserve">12P WINGS DINNER</t>
@@ -226,7 +214,7 @@
     <t xml:space="preserve">12P  WNG DIN</t>
   </si>
   <si>
-    <t xml:space="preserve">*Fries Reg, FRIED PICKLES</t>
+    <t xml:space="preserve">Fries Reg, FRIED PICKLES</t>
   </si>
   <si>
     <t xml:space="preserve">12P WINGS COMBO</t>
@@ -241,10 +229,10 @@
     <t xml:space="preserve">LgCmb 12P WNG</t>
   </si>
   <si>
-    <t xml:space="preserve">*Mash&amp;Gravy Re, COLESLAW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Lg Coke, SicomDrPepper</t>
+    <t xml:space="preserve">Mash&amp;Gravy Re, COLESLAW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lg Coke, DrPepper</t>
   </si>
 </sst>
 </file>
@@ -451,10 +439,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1048576"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -466,9 +454,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="25.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="25.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="12.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -502,34 +490,28 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,25 +519,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -563,28 +545,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -592,22 +574,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -615,28 +597,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -644,28 +623,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -673,22 +652,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -696,31 +675,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -728,34 +704,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -763,37 +733,31 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -801,22 +765,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -824,22 +788,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -847,22 +811,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -870,28 +834,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -899,31 +860,28 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -931,34 +889,31 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="I17" s="1" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -966,34 +921,31 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="I18" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Code clean-up and update on the scripts up until the receipts part
</commit_message>
<xml_diff>
--- a/Popeyes.suite/Resources/Sicom.xlsx
+++ b/Popeyes.suite/Resources/Sicom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="97">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -52,6 +52,21 @@
     <t xml:space="preserve">Drink</t>
   </si>
   <si>
+    <t xml:space="preserve">KDSMealDisplayName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExpoLabelDisplayName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReceiptDisplayName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SandSidesDessertsDisplayName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProteinDisplayName</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPICY CHICKEN SANDWICH ALA CARTE</t>
   </si>
   <si>
@@ -82,6 +97,12 @@
     <t xml:space="preserve">Fries Reg, HOMESTYLE MAC &amp; CHEESE</t>
   </si>
   <si>
+    <t xml:space="preserve">Spcy Sand DNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spicy Sand, Mac &amp; Chs Reg</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPICY CHICKEN SANDWICH COMBO</t>
   </si>
   <si>
@@ -94,6 +115,15 @@
     <t xml:space="preserve">Rg Coke, CHILLED MANGO LEMONADE</t>
   </si>
   <si>
+    <t xml:space="preserve">Spcy Sand CMB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spicy Sand, Mac &amp; Chs Reg, Chl Mango Lmd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, </t>
+  </si>
+  <si>
     <t xml:space="preserve">SPICY CHICKEN SANDWICH LARGE COMBO</t>
   </si>
   <si>
@@ -103,6 +133,12 @@
     <t xml:space="preserve">Spcy San LCMB</t>
   </si>
   <si>
+    <t xml:space="preserve">Spcy Sand LCMB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spicy Sand, Mash&amp;Gravy Reg, Beans&amp;Rice Reg, Lg Coke</t>
+  </si>
+  <si>
     <t xml:space="preserve">4PC BIC DINNER</t>
   </si>
   <si>
@@ -118,6 +154,9 @@
     <t xml:space="preserve">Biscuit, FRIED PICKLES, Mash&amp;Gravy Re, CAJUN FRIES</t>
   </si>
   <si>
+    <t xml:space="preserve">Wng Clsc, Breast Clsc, Fried Pickles, Fries Reg</t>
+  </si>
+  <si>
     <t xml:space="preserve">4PC BIC COMBO</t>
   </si>
   <si>
@@ -130,48 +169,66 @@
     <t xml:space="preserve">Rg Coke, OrangeFanta</t>
   </si>
   <si>
+    <t xml:space="preserve">Wng Clsc, Breast Clsc, Biscuit, Fries Reg, Rg Orange</t>
+  </si>
+  <si>
     <t xml:space="preserve">4PC BIC LARGE COMBO</t>
   </si>
   <si>
     <t xml:space="preserve">LgCmb 4PC BIC</t>
   </si>
   <si>
+    <t xml:space="preserve">Wng Clsc, Breast Clsc, Biscuit, Mash&amp;Gravy Reg, Mash&amp;Gravy Reg, Lg Coke</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHRIMP AND 2 TENDERS ALA CARTE CUST</t>
   </si>
   <si>
     <t xml:space="preserve">SANDWICHES &amp; SEAFOOD, TO SEAFOOD</t>
   </si>
   <si>
+    <t xml:space="preserve">A LA CARTE, BTTRFLY SHRIMP &amp; TENDERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A LA CARTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSHRIMP&amp;TENDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cocktail, PICKLE, BBQ, BTTRMLK RANCH SAUCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tndr Clsc, SPICY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shrmp Bfly 4P, Tndr Clsc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHRIMP AND 2 TENDERS DINNER CUST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DINNER, BTTRFLY SHRIMP &amp; TENDERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSHRIMP&amp;TND DNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cocktail, POPEYES, BBQ, SWEET HEAT SAUCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tndr Clsc, SPICY, Mash&amp;Gravy Re, RED BEAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shrmp Bfly 4P, Tndr Spcy, Biscuit, Beans&amp;Rice Reg,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHRIMP AND 2 TENDERS COMBO CUST</t>
+  </si>
+  <si>
     <t xml:space="preserve">COMBO, BTTRFLY SHRIMP &amp; TENDERS</t>
   </si>
   <si>
-    <t xml:space="preserve">A LA CARTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BSHRIMP&amp;TENDER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cocktail, PICKLE, BBQ, BTTRMLK RANCH SAUCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tndr Clsc, SPICY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHRIMP AND 2 TENDERS DINNER CUST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BSHRIMP&amp;TND DNR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cocktail, TARTAR, BBQ, SWEET HEAT SAUCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tndr Clsc, SPICY, Mash&amp;Gravy Re, RED BEAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHRIMP AND 2 TENDERS COMBO CUST</t>
-  </si>
-  <si>
     <t xml:space="preserve">BSHRIMP&amp;TND CMB</t>
   </si>
   <si>
@@ -181,7 +238,7 @@
     <t xml:space="preserve">Tndr Clsc, SPICY, Mash&amp;Gravy Re, CAJUN FRIES</t>
   </si>
   <si>
-    <t xml:space="preserve">Rg Coke, DietCoke</t>
+    <t xml:space="preserve">Rg Coke, STARRY</t>
   </si>
   <si>
     <t xml:space="preserve">SHRIMP AND 2 TENDERS ALA CARTE</t>
@@ -190,9 +247,15 @@
     <t xml:space="preserve">SHRIMP AND 2 TENDERS DINNER</t>
   </si>
   <si>
+    <t xml:space="preserve">Shrmp Bfly 4P, Tndr  Clsc, Biscuit</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHRIMP AND 2 TENDERS COMBO</t>
   </si>
   <si>
+    <t xml:space="preserve">Shrmp Bfly 4P, Tndr Clsc, Biscuit, Mash&amp;Gravy Reg, Rg Coke</t>
+  </si>
+  <si>
     <t xml:space="preserve">12P WINGS</t>
   </si>
   <si>
@@ -208,6 +271,9 @@
     <t xml:space="preserve">Btrmlk Ranch, BBQ SAUCE, Btrmlk Ranch, BUFFALO SAUCE</t>
   </si>
   <si>
+    <t xml:space="preserve">WNG LmnPpr 6p, WNG HnyBbq 6P</t>
+  </si>
+  <si>
     <t xml:space="preserve">12P WINGS DINNER</t>
   </si>
   <si>
@@ -217,12 +283,21 @@
     <t xml:space="preserve">Fries Reg, FRIED PICKLES</t>
   </si>
   <si>
+    <t xml:space="preserve">12P WNG DIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WNG LmnPpr 6p, WNG HnyBbq 6P, Fried Pickles</t>
+  </si>
+  <si>
     <t xml:space="preserve">12P WINGS COMBO</t>
   </si>
   <si>
     <t xml:space="preserve">12P WNG Cmb</t>
   </si>
   <si>
+    <t xml:space="preserve">WNG LmnPpr 6p, WNG HnyBbq 6P, Mac &amp; Chs Reg</t>
+  </si>
+  <si>
     <t xml:space="preserve">12P WINGS LARGE COMBO</t>
   </si>
   <si>
@@ -233,6 +308,9 @@
   </si>
   <si>
     <t xml:space="preserve">Lg Coke, DrPepper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WNG LmnPpr 6p, WNG HnyBbq 6P, fFries Reg, Coleslaw Reg</t>
   </si>
 </sst>
 </file>
@@ -248,6 +326,7 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -439,10 +518,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1048576"/>
+  <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M18" activeCellId="0" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -456,10 +535,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="25.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="12.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="12.31"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,274 +572,352 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>24</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>36</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>48</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>59</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>65</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -765,22 +925,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>42</v>
+        <v>57</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -788,22 +954,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>46</v>
+        <v>63</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="O13" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -811,22 +983,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>50</v>
+        <v>69</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="O14" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -834,25 +1012,31 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>61</v>
+        <v>82</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -860,28 +1044,34 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>64</v>
+        <v>86</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="O16" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -889,31 +1079,37 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="O17" s="0" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -921,31 +1117,37 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>70</v>
+        <v>95</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="O18" s="0" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
started on receipt validation
</commit_message>
<xml_diff>
--- a/Popeyes.suite/Resources/Sicom.xlsx
+++ b/Popeyes.suite/Resources/Sicom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="103">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -85,6 +85,9 @@
     <t xml:space="preserve">Spicy Sand</t>
   </si>
   <si>
+    <t xml:space="preserve">Spicy Sandwich</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPICY CHICKEN SANDWICH DINNER</t>
   </si>
   <si>
@@ -118,9 +121,6 @@
     <t xml:space="preserve">Spcy Sand CMB</t>
   </si>
   <si>
-    <t xml:space="preserve">Spicy Sand, Mac &amp; Chs Reg, Chl Mango Lmd</t>
-  </si>
-  <si>
     <t xml:space="preserve">, </t>
   </si>
   <si>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">Spcy Sand LCMB</t>
   </si>
   <si>
-    <t xml:space="preserve">Spicy Sand, Mash&amp;Gravy Reg, Beans&amp;Rice Reg, Lg Coke</t>
+    <t xml:space="preserve">Spicy Sand, Mash&amp;Gravy Reg, Beans&amp;Rice Reg</t>
   </si>
   <si>
     <t xml:space="preserve">4PC BIC DINNER</t>
@@ -154,7 +154,13 @@
     <t xml:space="preserve">Biscuit, FRIED PICKLES, Mash&amp;Gravy Re, CAJUN FRIES</t>
   </si>
   <si>
-    <t xml:space="preserve">Wng Clsc, Breast Clsc, Fried Pickles, Fries Reg</t>
+    <t xml:space="preserve">Classic Wing, Classic Breast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fried Pickles, Fries Reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wng Clsc, Breast Clsc</t>
   </si>
   <si>
     <t xml:space="preserve">4PC BIC COMBO</t>
@@ -169,7 +175,7 @@
     <t xml:space="preserve">Rg Coke, OrangeFanta</t>
   </si>
   <si>
-    <t xml:space="preserve">Wng Clsc, Breast Clsc, Biscuit, Fries Reg, Rg Orange</t>
+    <t xml:space="preserve">Fries Reg</t>
   </si>
   <si>
     <t xml:space="preserve">4PC BIC LARGE COMBO</t>
@@ -178,7 +184,7 @@
     <t xml:space="preserve">LgCmb 4PC BIC</t>
   </si>
   <si>
-    <t xml:space="preserve">Wng Clsc, Breast Clsc, Biscuit, Mash&amp;Gravy Reg, Mash&amp;Gravy Reg, Lg Coke</t>
+    <t xml:space="preserve">Mash&amp;Gravy Reg, Mash&amp;Gravy Reg,</t>
   </si>
   <si>
     <t xml:space="preserve">SHRIMP AND 2 TENDERS ALA CARTE CUST</t>
@@ -202,6 +208,9 @@
     <t xml:space="preserve">Tndr Clsc, SPICY</t>
   </si>
   <si>
+    <t xml:space="preserve">Butterfly Shrimp, Spicy Tender</t>
+  </si>
+  <si>
     <t xml:space="preserve">Shrmp Bfly 4P, Tndr Clsc</t>
   </si>
   <si>
@@ -220,7 +229,10 @@
     <t xml:space="preserve">Tndr Clsc, SPICY, Mash&amp;Gravy Re, RED BEAN</t>
   </si>
   <si>
-    <t xml:space="preserve">Shrmp Bfly 4P, Tndr Spcy, Biscuit, Beans&amp;Rice Reg,</t>
+    <t xml:space="preserve">Beans&amp;Rice Reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shrmp Bfly 4P, Tndr Spcy</t>
   </si>
   <si>
     <t xml:space="preserve">SHRIMP AND 2 TENDERS COMBO CUST</t>
@@ -244,18 +256,21 @@
     <t xml:space="preserve">SHRIMP AND 2 TENDERS ALA CARTE</t>
   </si>
   <si>
+    <t xml:space="preserve">Butterfly Shrimp, Classic Tender</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHRIMP AND 2 TENDERS DINNER</t>
   </si>
   <si>
-    <t xml:space="preserve">Shrmp Bfly 4P, Tndr  Clsc, Biscuit</t>
+    <t xml:space="preserve">Mash&amp;Gravy Reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shrmp Bfly 4P, Tndr  Clsc</t>
   </si>
   <si>
     <t xml:space="preserve">SHRIMP AND 2 TENDERS COMBO</t>
   </si>
   <si>
-    <t xml:space="preserve">Shrmp Bfly 4P, Tndr Clsc, Biscuit, Mash&amp;Gravy Reg, Rg Coke</t>
-  </si>
-  <si>
     <t xml:space="preserve">12P WINGS</t>
   </si>
   <si>
@@ -271,6 +286,9 @@
     <t xml:space="preserve">Btrmlk Ranch, BBQ SAUCE, Btrmlk Ranch, BUFFALO SAUCE</t>
   </si>
   <si>
+    <t xml:space="preserve">Honey Lemon Wings, Honey BBQ Wings</t>
+  </si>
+  <si>
     <t xml:space="preserve">WNG LmnPpr 6p, WNG HnyBbq 6P</t>
   </si>
   <si>
@@ -286,7 +304,7 @@
     <t xml:space="preserve">12P WNG DIN</t>
   </si>
   <si>
-    <t xml:space="preserve">WNG LmnPpr 6p, WNG HnyBbq 6P, Fried Pickles</t>
+    <t xml:space="preserve">Fried Pickles</t>
   </si>
   <si>
     <t xml:space="preserve">12P WINGS COMBO</t>
@@ -295,7 +313,7 @@
     <t xml:space="preserve">12P WNG Cmb</t>
   </si>
   <si>
-    <t xml:space="preserve">WNG LmnPpr 6p, WNG HnyBbq 6P, Mac &amp; Chs Reg</t>
+    <t xml:space="preserve">Mac &amp; Chs Reg</t>
   </si>
   <si>
     <t xml:space="preserve">12P WINGS LARGE COMBO</t>
@@ -310,7 +328,7 @@
     <t xml:space="preserve">Lg Coke, DrPepper</t>
   </si>
   <si>
-    <t xml:space="preserve">WNG LmnPpr 6p, WNG HnyBbq 6P, fFries Reg, Coleslaw Reg</t>
+    <t xml:space="preserve">Fries Reg, Coleslaw Reg</t>
   </si>
 </sst>
 </file>
@@ -320,7 +338,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -342,6 +360,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -386,12 +410,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -520,8 +548,8 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M18" activeCellId="0" sqref="M18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -613,6 +641,9 @@
       <c r="K2" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="M2" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="N2" s="0" t="s">
         <v>20</v>
       </c>
@@ -622,7 +653,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -634,19 +665,22 @@
         <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -654,7 +688,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
@@ -666,22 +700,25 @@
         <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="O4" s="0" t="s">
         <v>33</v>
@@ -712,6 +749,9 @@
       <c r="K5" s="0" t="s">
         <v>37</v>
       </c>
+      <c r="M5" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="N5" s="0" t="s">
         <v>38</v>
       </c>
@@ -733,7 +773,7 @@
         <v>41</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>42</v>
@@ -744,8 +784,14 @@
       <c r="K6" s="0" t="s">
         <v>42</v>
       </c>
+      <c r="M6" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="O6" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -753,7 +799,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>16</v>
@@ -765,22 +811,28 @@
         <v>41</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="O7" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -788,7 +840,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>16</v>
@@ -803,13 +855,19 @@
         <v>35</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>54</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -817,34 +875,37 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="0" t="s">
-        <v>57</v>
+      <c r="M9" s="0" t="s">
+        <v>62</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -852,34 +913,40 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="M10" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>63</v>
+      <c r="N10" s="0" t="s">
+        <v>69</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -887,37 +954,43 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="O11" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="O11" s="0" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -925,28 +998,31 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>78</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -954,28 +1030,34 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>80</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -983,28 +1065,34 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>80</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1012,31 +1100,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1044,34 +1135,40 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>94</v>
       </c>
       <c r="O16" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1079,37 +1176,43 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N17" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="O17" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="O17" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1117,37 +1220,43 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N18" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
progress on receipt validation
</commit_message>
<xml_diff>
--- a/Popeyes.suite/Resources/Sicom.xlsx
+++ b/Popeyes.suite/Resources/Sicom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="104">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -142,45 +142,48 @@
     <t xml:space="preserve">4PC BIC DINNER</t>
   </si>
   <si>
+    <t xml:space="preserve">CHICKEN,4PC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL WHITE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4PC BIC Dinner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biscuit, FRIED PICKLES, Mash&amp;Gravy Re, CAJUN FRIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classic Wing, Classic Breast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fried Pickles, Fries Reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wng Clsc, Breast Clsc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4PC BIC COMBO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4PC BIC Combo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mash&amp;Gravy Re, CAJUN FRIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rg Coke, OrangeFanta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fries Reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4PC BIC LARGE COMBO</t>
+  </si>
+  <si>
     <t xml:space="preserve">CHICKEN, 4PC</t>
   </si>
   <si>
-    <t xml:space="preserve">ALL WHITE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4PC BIC Dinner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biscuit, FRIED PICKLES, Mash&amp;Gravy Re, CAJUN FRIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Classic Wing, Classic Breast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fried Pickles, Fries Reg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wng Clsc, Breast Clsc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4PC BIC COMBO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4PC BIC Combo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mash&amp;Gravy Re, CAJUN FRIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rg Coke, OrangeFanta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fries Reg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4PC BIC LARGE COMBO</t>
-  </si>
-  <si>
     <t xml:space="preserve">LgCmb 4PC BIC</t>
   </si>
   <si>
@@ -190,7 +193,7 @@
     <t xml:space="preserve">SHRIMP AND 2 TENDERS ALA CARTE CUST</t>
   </si>
   <si>
-    <t xml:space="preserve">SANDWICHES &amp; SEAFOOD, TO SEAFOOD</t>
+    <t xml:space="preserve">SANDWICHES &amp; SEAFOOD,TO SEAFOOD</t>
   </si>
   <si>
     <t xml:space="preserve">A LA CARTE, BTTRFLY SHRIMP &amp; TENDERS</t>
@@ -548,8 +551,8 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -846,7 +849,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>41</v>
@@ -855,16 +858,16 @@
         <v>35</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M8" s="0" t="s">
         <v>44</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O8" s="0" t="s">
         <v>46</v>
@@ -875,37 +878,37 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>59</v>
-      </c>
       <c r="M9" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -913,40 +916,40 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="M10" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -954,43 +957,43 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K11" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>73</v>
-      </c>
       <c r="M11" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N11" s="0" t="s">
         <v>51</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -998,31 +1001,31 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1030,34 +1033,34 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1065,34 +1068,34 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1100,34 +1103,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="G15" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K15" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="K15" s="0" t="s">
-        <v>86</v>
-      </c>
       <c r="M15" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1135,40 +1138,40 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="O16" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="N16" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="O16" s="0" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1176,25 +1179,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>25</v>
@@ -1203,16 +1206,16 @@
         <v>31</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O17" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1220,43 +1223,43 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K18" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>99</v>
-      </c>
       <c r="M18" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
changes on the handler
</commit_message>
<xml_diff>
--- a/Popeyes.suite/Resources/Sicom.xlsx
+++ b/Popeyes.suite/Resources/Sicom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="107">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -64,9 +64,15 @@
     <t xml:space="preserve">SandSidesDessertsDisplayName</t>
   </si>
   <si>
+    <t xml:space="preserve">SidesValidation</t>
+  </si>
+  <si>
     <t xml:space="preserve">ProteinDisplayName</t>
   </si>
   <si>
+    <t xml:space="preserve">ProteinValidation</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPICY CHICKEN SANDWICH ALA CARTE</t>
   </si>
   <si>
@@ -88,6 +94,12 @@
     <t xml:space="preserve">Spicy Sandwich</t>
   </si>
   <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPICY CHICKEN SANDWICH DINNER</t>
   </si>
   <si>
@@ -179,9 +191,6 @@
   </si>
   <si>
     <t xml:space="preserve">4PC BIC LARGE COMBO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHICKEN, 4PC</t>
   </si>
   <si>
     <t xml:space="preserve">LgCmb 4PC BIC</t>
@@ -549,10 +558,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O1048576"/>
+  <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="R15" activeCellId="0" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -569,7 +578,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="12.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="12.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -618,37 +627,49 @@
       <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -656,34 +677,40 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="N3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -691,40 +718,46 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q4" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,31 +765,37 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -764,37 +803,43 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O6" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -802,40 +847,46 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="N7" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="K7" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="N7" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>46</v>
+      <c r="Q7" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -843,34 +894,40 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>46</v>
+        <v>24</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q8" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,37 +935,43 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>64</v>
+        <v>25</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q9" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -916,40 +979,46 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="M10" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="M10" s="0" t="s">
-        <v>63</v>
-      </c>
       <c r="N10" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>71</v>
+        <v>24</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q10" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -957,43 +1026,49 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="P11" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="M11" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="N11" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="O11" s="0" t="s">
-        <v>71</v>
+      <c r="Q11" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1001,31 +1076,37 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>64</v>
+        <v>25</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q12" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1033,34 +1114,40 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>82</v>
+        <v>24</v>
+      </c>
+      <c r="P13" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q13" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1068,34 +1155,40 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>64</v>
+        <v>24</v>
+      </c>
+      <c r="P14" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q14" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1103,34 +1196,40 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>90</v>
+        <v>25</v>
+      </c>
+      <c r="P15" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q15" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1138,40 +1237,46 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G16" s="1" t="s">
+      <c r="I16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="M16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I16" s="1" t="s">
+      <c r="N16" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="O16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="P16" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="K16" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="N16" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="O16" s="0" t="s">
-        <v>90</v>
+      <c r="Q16" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1179,43 +1284,49 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="O17" s="0" t="s">
-        <v>90</v>
+        <v>24</v>
+      </c>
+      <c r="P17" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q17" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1223,43 +1334,49 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>90</v>
+        <v>24</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q18" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
adding updates for Receipt Validation
</commit_message>
<xml_diff>
--- a/Popeyes.suite/Resources/Sicom.xlsx
+++ b/Popeyes.suite/Resources/Sicom.xlsx
@@ -350,7 +350,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -372,12 +372,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -431,7 +425,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -560,8 +554,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R15" activeCellId="0" sqref="R15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -575,9 +569,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="25.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="12.31"/>
   </cols>
   <sheetData>
@@ -612,25 +606,25 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -656,19 +650,19 @@
       <c r="G2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="N2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="0" t="s">
+      <c r="O2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -697,19 +691,19 @@
       <c r="I3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="N3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q3" s="0" t="s">
+      <c r="O3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -741,22 +735,22 @@
       <c r="J4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="M4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="N4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" s="0" t="s">
+      <c r="O4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="Q4" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -782,19 +776,19 @@
       <c r="G5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="K5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="0" t="s">
+      <c r="M5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N5" s="0" t="s">
+      <c r="N5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q5" s="0" t="s">
+      <c r="O5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -823,10 +817,10 @@
       <c r="I6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="K6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="M6" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N6" s="2" t="s">
@@ -835,10 +829,10 @@
       <c r="O6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="P6" s="0" t="s">
+      <c r="P6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="Q6" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -870,22 +864,22 @@
       <c r="J7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="K7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M7" s="0" t="s">
+      <c r="M7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="N7" s="0" t="s">
+      <c r="N7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O7" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="P7" s="0" t="s">
+      <c r="O7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="Q7" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -911,22 +905,22 @@
       <c r="G8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="K8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M8" s="0" t="s">
+      <c r="M8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="N8" s="0" t="s">
+      <c r="N8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="O8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="P8" s="0" t="s">
+      <c r="O8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q8" s="0" t="s">
+      <c r="Q8" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -958,19 +952,19 @@
       <c r="I9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K9" s="0" t="s">
+      <c r="K9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="M9" s="0" t="s">
+      <c r="M9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O9" s="0" t="s">
+      <c r="O9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P9" s="0" t="s">
+      <c r="P9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q9" s="0" t="s">
+      <c r="Q9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1002,22 +996,22 @@
       <c r="I10" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K10" s="0" t="s">
+      <c r="K10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M10" s="0" t="s">
+      <c r="M10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N10" s="0" t="s">
+      <c r="N10" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="O10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="P10" s="0" t="s">
+      <c r="O10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Q10" s="0" t="s">
+      <c r="Q10" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1052,22 +1046,22 @@
       <c r="J11" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="K11" s="0" t="s">
+      <c r="K11" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="M11" s="0" t="s">
+      <c r="M11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N11" s="0" t="s">
+      <c r="N11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O11" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="P11" s="0" t="s">
+      <c r="O11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Q11" s="0" t="s">
+      <c r="Q11" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1093,19 +1087,19 @@
       <c r="G12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K12" s="0" t="s">
+      <c r="K12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="M12" s="0" t="s">
+      <c r="M12" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O12" s="0" t="s">
+      <c r="O12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P12" s="0" t="s">
+      <c r="P12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q12" s="0" t="s">
+      <c r="Q12" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1131,22 +1125,22 @@
       <c r="G13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="K13" s="0" t="s">
+      <c r="K13" s="1" t="s">
         <v>70</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="N13" s="0" t="s">
+      <c r="N13" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="O13" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="P13" s="0" t="s">
+      <c r="O13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="Q13" s="0" t="s">
+      <c r="Q13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1172,22 +1166,22 @@
       <c r="G14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K14" s="0" t="s">
+      <c r="K14" s="1" t="s">
         <v>77</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="N14" s="0" t="s">
+      <c r="N14" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="O14" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="P14" s="0" t="s">
+      <c r="O14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q14" s="0" t="s">
+      <c r="Q14" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1216,19 +1210,19 @@
       <c r="H15" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K15" s="0" t="s">
+      <c r="K15" s="1" t="s">
         <v>90</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="O15" s="0" t="s">
+      <c r="O15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P15" s="0" t="s">
+      <c r="P15" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q15" s="0" t="s">
+      <c r="Q15" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1260,22 +1254,22 @@
       <c r="I16" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K16" s="0" t="s">
+      <c r="K16" s="1" t="s">
         <v>97</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="N16" s="0" t="s">
+      <c r="N16" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="O16" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="P16" s="0" t="s">
+      <c r="O16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P16" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q16" s="0" t="s">
+      <c r="Q16" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1310,22 +1304,22 @@
       <c r="J17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="0" t="s">
+      <c r="K17" s="1" t="s">
         <v>100</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="N17" s="0" t="s">
+      <c r="N17" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="O17" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="P17" s="0" t="s">
+      <c r="O17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P17" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q17" s="0" t="s">
+      <c r="Q17" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1360,22 +1354,22 @@
       <c r="J18" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K18" s="0" t="s">
+      <c r="K18" s="1" t="s">
         <v>103</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="N18" s="0" t="s">
+      <c r="N18" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="O18" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="P18" s="0" t="s">
+      <c r="O18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P18" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q18" s="0" t="s">
+      <c r="Q18" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final updates and changes
</commit_message>
<xml_diff>
--- a/Popeyes.suite/Resources/Sicom.xlsx
+++ b/Popeyes.suite/Resources/Sicom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="109">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">ProteinValidation</t>
   </si>
   <si>
-    <t xml:space="preserve">SPICY CHICKEN SANDWICH ALA CARTE</t>
+    <t xml:space="preserve">Spicy Chicken Sandwich ALC</t>
   </si>
   <si>
     <t xml:space="preserve">Dine In</t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">NO</t>
   </si>
   <si>
-    <t xml:space="preserve">SPICY CHICKEN SANDWICH DINNER</t>
+    <t xml:space="preserve">Spicy Chicken Sandwich Dinner</t>
   </si>
   <si>
     <t xml:space="preserve">DINNER</t>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">Spicy Sand, Mac &amp; Chs Reg</t>
   </si>
   <si>
-    <t xml:space="preserve">SPICY CHICKEN SANDWICH COMBO</t>
+    <t xml:space="preserve">Spicy Chicken Sandwich Combo</t>
   </si>
   <si>
     <t xml:space="preserve">COMBO</t>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">, </t>
   </si>
   <si>
-    <t xml:space="preserve">SPICY CHICKEN SANDWICH LARGE COMBO</t>
+    <t xml:space="preserve">Spicy Chicken Sandwich Large Combo</t>
   </si>
   <si>
     <t xml:space="preserve">LARGE COMBO</t>
@@ -151,7 +151,7 @@
     <t xml:space="preserve">Spicy Sand, Mash&amp;Gravy Reg, Beans&amp;Rice Reg</t>
   </si>
   <si>
-    <t xml:space="preserve">4PC BIC DINNER</t>
+    <t xml:space="preserve">4PC BIC Dinner</t>
   </si>
   <si>
     <t xml:space="preserve">CHICKEN,4PC</t>
@@ -160,9 +160,6 @@
     <t xml:space="preserve">ALL WHITE</t>
   </si>
   <si>
-    <t xml:space="preserve">4PC BIC Dinner</t>
-  </si>
-  <si>
     <t xml:space="preserve">Biscuit, FRIED PICKLES, Mash&amp;Gravy Re, CAJUN FRIES</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
     <t xml:space="preserve">Wng Clsc, Breast Clsc</t>
   </si>
   <si>
-    <t xml:space="preserve">4PC BIC COMBO</t>
-  </si>
-  <si>
     <t xml:space="preserve">4PC BIC Combo</t>
   </si>
   <si>
@@ -190,7 +184,7 @@
     <t xml:space="preserve">Fries Reg</t>
   </si>
   <si>
-    <t xml:space="preserve">4PC BIC LARGE COMBO</t>
+    <t xml:space="preserve">4PC BIC Large Combo</t>
   </si>
   <si>
     <t xml:space="preserve">LgCmb 4PC BIC</t>
@@ -199,7 +193,7 @@
     <t xml:space="preserve">Mash&amp;Gravy Reg, Mash&amp;Gravy Reg,</t>
   </si>
   <si>
-    <t xml:space="preserve">SHRIMP AND 2 TENDERS ALA CARTE CUST</t>
+    <t xml:space="preserve">Shrimp and 2 Tenders ALC Cust</t>
   </si>
   <si>
     <t xml:space="preserve">SANDWICHES &amp; SEAFOOD,TO SEAFOOD</t>
@@ -223,10 +217,10 @@
     <t xml:space="preserve">Butterfly Shrimp, Spicy Tender</t>
   </si>
   <si>
-    <t xml:space="preserve">Shrmp Bfly 4P, Tndr Clsc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHRIMP AND 2 TENDERS DINNER CUST</t>
+    <t xml:space="preserve">Tndr Clsc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shrimp and 2 Tenders Dinner Cust</t>
   </si>
   <si>
     <t xml:space="preserve">DINNER, BTTRFLY SHRIMP &amp; TENDERS</t>
@@ -244,10 +238,10 @@
     <t xml:space="preserve">Beans&amp;Rice Reg</t>
   </si>
   <si>
-    <t xml:space="preserve">Shrmp Bfly 4P, Tndr Spcy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHRIMP AND 2 TENDERS COMBO CUST</t>
+    <t xml:space="preserve">Tndr Spcy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shrimp and 2 Tenders Combo Cust</t>
   </si>
   <si>
     <t xml:space="preserve">COMBO, BTTRFLY SHRIMP &amp; TENDERS</t>
@@ -265,33 +259,36 @@
     <t xml:space="preserve">Rg Coke, STARRY</t>
   </si>
   <si>
-    <t xml:space="preserve">SHRIMP AND 2 TENDERS ALA CARTE</t>
+    <t xml:space="preserve">Shrimp and 2 Tenders ALC</t>
   </si>
   <si>
     <t xml:space="preserve">Butterfly Shrimp, Classic Tender</t>
   </si>
   <si>
-    <t xml:space="preserve">SHRIMP AND 2 TENDERS DINNER</t>
+    <t xml:space="preserve">Shrimp and 2 Tenders Dinner</t>
   </si>
   <si>
     <t xml:space="preserve">Mash&amp;Gravy Reg</t>
   </si>
   <si>
-    <t xml:space="preserve">Shrmp Bfly 4P, Tndr  Clsc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHRIMP AND 2 TENDERS COMBO</t>
+    <t xml:space="preserve">Tndr  Clsc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shrimp and 2 Tenders Combo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12P Wings ALC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WINGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6P HONEY LEMON WINGS, 6P HONEY BBQ WINGS</t>
   </si>
   <si>
     <t xml:space="preserve">12P WINGS</t>
   </si>
   <si>
-    <t xml:space="preserve">WINGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6P HONEY LEMON WINGS, 6P HONEY BBQ WINGS</t>
-  </si>
-  <si>
     <t xml:space="preserve">12P WNG</t>
   </si>
   <si>
@@ -304,6 +301,9 @@
     <t xml:space="preserve">WNG LmnPpr 6p, WNG HnyBbq 6P</t>
   </si>
   <si>
+    <t xml:space="preserve">12P Wings Dinner</t>
+  </si>
+  <si>
     <t xml:space="preserve">12P WINGS DINNER</t>
   </si>
   <si>
@@ -319,6 +319,9 @@
     <t xml:space="preserve">Fried Pickles</t>
   </si>
   <si>
+    <t xml:space="preserve">12P Wings Combo</t>
+  </si>
+  <si>
     <t xml:space="preserve">12P WINGS COMBO</t>
   </si>
   <si>
@@ -326,6 +329,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mac &amp; Chs Reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12P Wings Large Combo</t>
   </si>
   <si>
     <t xml:space="preserve">12P WINGS LARGE COMBO</t>
@@ -554,8 +560,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P20" activeCellId="0" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -812,25 +818,25 @@
         <v>27</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="K6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="O6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>24</v>
@@ -841,7 +847,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
@@ -856,28 +862,28 @@
         <v>33</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="K7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="O7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>24</v>
@@ -888,7 +894,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
@@ -903,22 +909,22 @@
         <v>39</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q8" s="1" t="s">
         <v>24</v>
@@ -929,40 +935,40 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="K9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>24</v>
@@ -973,43 +979,43 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="K10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="O10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>24</v>
@@ -1020,46 +1026,46 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="K11" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>24</v>
@@ -1070,34 +1076,34 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="K12" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>24</v>
@@ -1108,37 +1114,37 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="O13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q13" s="1" t="s">
         <v>24</v>
@@ -1149,37 +1155,37 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="O14" s="1" t="s">
         <v>24</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>24</v>
@@ -1190,37 +1196,37 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="K15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M15" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>25</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>24</v>
@@ -1231,16 +1237,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>94</v>
@@ -1249,7 +1255,7 @@
         <v>95</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>96</v>
@@ -1258,7 +1264,7 @@
         <v>97</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>98</v>
@@ -1267,7 +1273,7 @@
         <v>24</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>24</v>
@@ -1284,19 +1290,19 @@
         <v>18</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>29</v>
@@ -1305,19 +1311,19 @@
         <v>35</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="M17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P17" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="Q17" s="1" t="s">
         <v>24</v>
@@ -1328,46 +1334,46 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="M18" s="2" t="s">
+      <c r="N18" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P18" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="Q18" s="1" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Committing changes for app scripts before pull
</commit_message>
<xml_diff>
--- a/Popeyes.suite/Resources/Sicom.xlsx
+++ b/Popeyes.suite/Resources/Sicom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="112">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -347,6 +347,15 @@
   </si>
   <si>
     <t xml:space="preserve">Fries Reg, Coleslaw Reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coupon Look Up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Butterfly Shrimp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X Off</t>
   </si>
 </sst>
 </file>
@@ -560,8 +569,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P20" activeCellId="0" sqref="P20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N21" activeCellId="0" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1379,6 +1388,79 @@
         <v>24</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N19" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="O19" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q19" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P20" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q20" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Push for Delivery 4
</commit_message>
<xml_diff>
--- a/Popeyes.suite/Resources/Sicom.xlsx
+++ b/Popeyes.suite/Resources/Sicom.xlsx
@@ -349,13 +349,13 @@
     <t xml:space="preserve">Fries Reg, Coleslaw Reg</t>
   </si>
   <si>
-    <t xml:space="preserve">Coupon Look Up</t>
+    <t xml:space="preserve">PLU Lookup</t>
   </si>
   <si>
     <t xml:space="preserve">Butterfly Shrimp</t>
   </si>
   <si>
-    <t xml:space="preserve">X Off</t>
+    <t xml:space="preserve">X% Off Discount</t>
   </si>
 </sst>
 </file>
@@ -569,8 +569,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N21" activeCellId="0" sqref="N21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1395,7 +1395,7 @@
       <c r="B19" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1416,13 +1416,13 @@
       <c r="M19" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="N19" s="0" t="s">
+      <c r="N19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O19" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q19" s="0" t="s">
+      <c r="O19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q19" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1433,7 +1433,7 @@
       <c r="B20" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1454,10 +1454,10 @@
       <c r="M20" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="P20" s="0" t="s">
+      <c r="P20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Q20" s="0" t="s">
+      <c r="Q20" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>